<commit_message>
avec OSC pour ESP32
</commit_message>
<xml_diff>
--- a/pieces/Les pièces Skini.xlsx
+++ b/pieces/Les pièces Skini.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berpetit.AD\Documents\nodeskini\pieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5BDED3C-3889-47B0-803F-C709FE88D8F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781D17B9-19BD-47EE-B76D-B6380E3A6F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="-840" windowWidth="30270" windowHeight="14805" xr2:uid="{6D6D9BFB-4BA4-4FFE-8AC7-F35E8058755B}"/>
+    <workbookView xWindow="-26970" yWindow="-3000" windowWidth="25275" windowHeight="14805" xr2:uid="{6D6D9BFB-4BA4-4FFE-8AC7-F35E8058755B}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="234">
   <si>
     <t>opus1 skini V2-ABL10.als</t>
   </si>
@@ -546,9 +546,6 @@
     <t>Pour trio à corde avec sélection des articulation des cordes via midiconveter dans les patterns</t>
   </si>
   <si>
-    <t>Version du 19/4/2022</t>
-  </si>
-  <si>
     <t>Pièces Bitwig Studio NodeSkini</t>
   </si>
   <si>
@@ -564,15 +561,6 @@
     <t>Pour démo techno, percu, musique du monde</t>
   </si>
   <si>
-    <t>PIECES AVEC 3 AUTOMATES - Skini Hop.js</t>
-  </si>
-  <si>
-    <t>PIECES AVEC UN SEUL AUTOMATE - Skini Hop.js</t>
-  </si>
-  <si>
-    <t>JEUX MUSICAUX - Skini Hop.js</t>
-  </si>
-  <si>
     <t>Beaucoup d'évolutions techniques par rapport à Hop.js: plus d'automate en dehors de Blockly, différentes synchro possibles, pas de pièce au lancement, simulateur intégré…</t>
   </si>
   <si>
@@ -703,13 +691,55 @@
   </si>
   <si>
     <t>DMF, tanks, transposition et mvt de tempo avec simulateur en -sim</t>
+  </si>
+  <si>
+    <t>opus4.hh.js</t>
+  </si>
+  <si>
+    <t>non</t>
+  </si>
+  <si>
+    <t>reprise d'opus4 en programmation HH avec possibilité de capteurs IZ</t>
+  </si>
+  <si>
+    <t>capteursIZ.hh.js</t>
+  </si>
+  <si>
+    <t>TestCapteursIZ.als</t>
+  </si>
+  <si>
+    <t>programme de test la boite des capteurs IZ</t>
+  </si>
+  <si>
+    <t>En programmation textuelle HipHop</t>
+  </si>
+  <si>
+    <t>capteursIZ.js</t>
+  </si>
+  <si>
+    <t>PIECES AVEC 3 AUTOMATES - Skini sur Hop.js (plus à jour en 2024)</t>
+  </si>
+  <si>
+    <t>JEUX MUSICAUX - Skini Hop.js (plus à jour en 2024)</t>
+  </si>
+  <si>
+    <t>PIECES AVEC UN SEUL AUTOMATE - Skini sur Hop.js (plus à jour en 2024)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Skini sur Node.js </t>
+  </si>
+  <si>
+    <t>En programmation graphique Blockly</t>
+  </si>
+  <si>
+    <t>Version du 30/5/2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -725,8 +755,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -790,6 +828,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -938,7 +982,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1048,6 +1092,9 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1362,12 +1409,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3771670C-3569-4306-BADE-9BE1604036BE}">
-  <dimension ref="A1:Y93"/>
+  <dimension ref="A1:Y98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A12" sqref="A12"/>
-      <selection pane="topRight" activeCell="J96" sqref="J96"/>
+      <selection pane="topRight" activeCell="C108" sqref="C108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1394,7 +1441,7 @@
   <sheetData>
     <row r="1" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>171</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
@@ -1750,7 +1797,7 @@
     </row>
     <row r="17" spans="1:25" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="54" t="s">
-        <v>177</v>
+        <v>228</v>
       </c>
       <c r="B17" s="54"/>
     </row>
@@ -2409,7 +2456,7 @@
     </row>
     <row r="47" spans="1:20" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="54" t="s">
-        <v>178</v>
+        <v>230</v>
       </c>
       <c r="B47" s="55"/>
     </row>
@@ -2705,7 +2752,7 @@
       <c r="I64" s="20"/>
       <c r="J64" s="21"/>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B65" s="25" t="s">
         <v>121</v>
       </c>
@@ -2728,13 +2775,13 @@
       <c r="I65" s="26"/>
       <c r="J65" s="27"/>
     </row>
-    <row r="67" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67" s="54" t="s">
-        <v>179</v>
+        <v>229</v>
       </c>
       <c r="B67" s="55"/>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A69" s="50" t="s">
         <v>137</v>
       </c>
@@ -2760,7 +2807,7 @@
       <c r="I69" s="31"/>
       <c r="J69" s="32"/>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>164</v>
       </c>
@@ -2786,7 +2833,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>13</v>
       </c>
@@ -2812,7 +2859,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>165</v>
       </c>
@@ -2838,7 +2885,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>166</v>
       </c>
@@ -2864,256 +2911,331 @@
         <v>163</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
       <c r="E74" s="23"/>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A75" s="58" t="s">
+    <row r="75" spans="1:14" ht="21" x14ac:dyDescent="0.4">
+      <c r="A75" s="62" t="s">
+        <v>231</v>
+      </c>
+      <c r="B75" s="55"/>
+      <c r="C75" s="10"/>
+      <c r="D75" s="10"/>
+      <c r="E75" s="10"/>
+      <c r="F75" s="10"/>
+      <c r="G75" s="10"/>
+      <c r="H75" s="10"/>
+      <c r="I75" s="10"/>
+      <c r="J75" s="10"/>
+      <c r="K75" s="10"/>
+      <c r="L75" s="10"/>
+      <c r="M75" s="10"/>
+      <c r="N75" s="10"/>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A76" s="61" t="s">
+        <v>232</v>
+      </c>
+      <c r="E76" s="23"/>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A77" s="58" t="s">
+        <v>171</v>
+      </c>
+      <c r="B77" s="59"/>
+      <c r="C77" s="59" t="s">
+        <v>176</v>
+      </c>
+      <c r="D77" s="59"/>
+      <c r="E77" s="59"/>
+      <c r="F77" s="59"/>
+      <c r="G77" s="59"/>
+      <c r="H77" s="59"/>
+      <c r="I77" s="59"/>
+      <c r="J77" s="60"/>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C78" t="s">
+        <v>167</v>
+      </c>
+      <c r="F78" s="57" t="s">
+        <v>169</v>
+      </c>
+      <c r="G78" t="s">
+        <v>168</v>
+      </c>
+      <c r="I78" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C79" t="s">
         <v>172</v>
       </c>
-      <c r="B75" s="59"/>
-      <c r="C75" s="59" t="s">
+      <c r="F79" t="s">
+        <v>173</v>
+      </c>
+      <c r="G79" t="s">
+        <v>174</v>
+      </c>
+      <c r="I79" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C80" t="s">
+        <v>179</v>
+      </c>
+      <c r="F80" t="s">
+        <v>181</v>
+      </c>
+      <c r="G80" t="s">
+        <v>177</v>
+      </c>
+      <c r="I80" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C81" t="s">
         <v>180</v>
       </c>
-      <c r="D75" s="59"/>
-      <c r="E75" s="59"/>
-      <c r="F75" s="59"/>
-      <c r="G75" s="59"/>
-      <c r="H75" s="59"/>
-      <c r="I75" s="59"/>
-      <c r="J75" s="60"/>
-    </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C76" t="s">
-        <v>167</v>
-      </c>
-      <c r="F76" s="57" t="s">
+      <c r="F81" t="s">
+        <v>181</v>
+      </c>
+      <c r="G81" t="s">
+        <v>178</v>
+      </c>
+      <c r="I81" t="s">
+        <v>201</v>
+      </c>
+      <c r="M81" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C82" t="s">
+        <v>148</v>
+      </c>
+      <c r="F82" t="s">
+        <v>140</v>
+      </c>
+      <c r="G82" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C83" t="s">
+        <v>192</v>
+      </c>
+      <c r="F83" s="57" t="s">
         <v>169</v>
       </c>
-      <c r="G76" t="s">
-        <v>168</v>
-      </c>
-      <c r="I76" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C77" t="s">
-        <v>173</v>
-      </c>
-      <c r="F77" t="s">
-        <v>174</v>
-      </c>
-      <c r="G77" t="s">
-        <v>175</v>
-      </c>
-      <c r="I77" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C78" t="s">
-        <v>183</v>
-      </c>
-      <c r="F78" t="s">
+      <c r="G83" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C84" t="s">
+        <v>203</v>
+      </c>
+      <c r="F84" t="s">
+        <v>202</v>
+      </c>
+      <c r="G84" t="s">
+        <v>204</v>
+      </c>
+      <c r="I84" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C85" t="s">
+        <v>193</v>
+      </c>
+      <c r="F85" t="s">
+        <v>194</v>
+      </c>
+      <c r="G85" t="s">
+        <v>196</v>
+      </c>
+      <c r="I85" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A87" s="58" t="s">
+        <v>187</v>
+      </c>
+      <c r="B87" s="59"/>
+      <c r="C87" s="59"/>
+      <c r="D87" s="59"/>
+      <c r="E87" s="59"/>
+      <c r="F87" s="59"/>
+      <c r="G87" s="59"/>
+      <c r="H87" s="59"/>
+      <c r="I87" s="59"/>
+      <c r="J87" s="59"/>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C88" t="s">
+        <v>186</v>
+      </c>
+      <c r="F88" t="s">
+        <v>184</v>
+      </c>
+      <c r="G88" t="s">
         <v>185</v>
       </c>
-      <c r="G78" t="s">
-        <v>181</v>
-      </c>
-      <c r="I78" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C79" t="s">
-        <v>184</v>
-      </c>
-      <c r="F79" t="s">
-        <v>185</v>
-      </c>
-      <c r="G79" t="s">
-        <v>182</v>
-      </c>
-      <c r="I79" t="s">
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C89" t="s">
+        <v>88</v>
+      </c>
+      <c r="F89" t="s">
+        <v>3</v>
+      </c>
+      <c r="G89" t="s">
+        <v>188</v>
+      </c>
+      <c r="I89" t="s">
+        <v>189</v>
+      </c>
+      <c r="K89" t="s">
         <v>205</v>
       </c>
-      <c r="M79" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C80" t="s">
-        <v>148</v>
-      </c>
-      <c r="F80" t="s">
-        <v>140</v>
-      </c>
-      <c r="G80" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C81" t="s">
-        <v>196</v>
-      </c>
-      <c r="F81" s="57" t="s">
-        <v>169</v>
-      </c>
-      <c r="G81" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C82" t="s">
-        <v>207</v>
-      </c>
-      <c r="F82" t="s">
-        <v>206</v>
-      </c>
-      <c r="G82" t="s">
-        <v>208</v>
-      </c>
-      <c r="I82" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C83" t="s">
-        <v>197</v>
-      </c>
-      <c r="F83" t="s">
-        <v>198</v>
-      </c>
-      <c r="G83" t="s">
-        <v>200</v>
-      </c>
-      <c r="I83" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A85" s="58" t="s">
-        <v>191</v>
-      </c>
-      <c r="B85" s="59"/>
-      <c r="C85" s="59"/>
-      <c r="D85" s="59"/>
-      <c r="E85" s="59"/>
-      <c r="F85" s="59"/>
-      <c r="G85" s="59"/>
-      <c r="H85" s="59"/>
-      <c r="I85" s="59"/>
-      <c r="J85" s="59"/>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C86" t="s">
-        <v>190</v>
-      </c>
-      <c r="F86" t="s">
-        <v>188</v>
-      </c>
-      <c r="G86" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C87" t="s">
-        <v>88</v>
-      </c>
-      <c r="F87" t="s">
-        <v>3</v>
-      </c>
-      <c r="G87" t="s">
-        <v>192</v>
-      </c>
-      <c r="I87" t="s">
-        <v>193</v>
-      </c>
-      <c r="K87" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C88" t="s">
-        <v>211</v>
-      </c>
-      <c r="F88" t="s">
-        <v>210</v>
-      </c>
-      <c r="G88" t="s">
-        <v>195</v>
-      </c>
-      <c r="I88" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C89" t="s">
-        <v>202</v>
-      </c>
-      <c r="F89" t="s">
-        <v>201</v>
-      </c>
-      <c r="G89" t="s">
-        <v>203</v>
-      </c>
-      <c r="I89" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C90" t="s">
         <v>207</v>
       </c>
       <c r="F90" t="s">
+        <v>206</v>
+      </c>
+      <c r="G90" t="s">
+        <v>191</v>
+      </c>
+      <c r="I90" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C91" t="s">
+        <v>198</v>
+      </c>
+      <c r="F91" t="s">
+        <v>197</v>
+      </c>
+      <c r="G91" t="s">
+        <v>199</v>
+      </c>
+      <c r="I91" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C92" t="s">
+        <v>203</v>
+      </c>
+      <c r="F92" t="s">
+        <v>209</v>
+      </c>
+      <c r="G92" t="s">
+        <v>204</v>
+      </c>
+      <c r="I92" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C93" t="s">
+        <v>203</v>
+      </c>
+      <c r="G93" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C94" t="s">
         <v>213</v>
       </c>
-      <c r="G90" t="s">
+      <c r="F94" t="s">
+        <v>212</v>
+      </c>
+      <c r="G94" t="s">
+        <v>214</v>
+      </c>
+      <c r="I94" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C95" t="s">
+        <v>216</v>
+      </c>
+      <c r="F95" t="s">
+        <v>218</v>
+      </c>
+      <c r="G95" t="s">
+        <v>217</v>
+      </c>
+      <c r="I95" t="s">
         <v>208</v>
       </c>
-      <c r="I90" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C91" t="s">
-        <v>207</v>
-      </c>
-      <c r="G91" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C92" t="s">
-        <v>217</v>
-      </c>
-      <c r="F92" t="s">
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A96" s="61" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>220</v>
+      </c>
+      <c r="B97" t="s">
+        <v>121</v>
+      </c>
+      <c r="C97" t="s">
+        <v>120</v>
+      </c>
+      <c r="F97" t="s">
+        <v>206</v>
+      </c>
+      <c r="G97" t="s">
+        <v>221</v>
+      </c>
+      <c r="I97" t="s">
+        <v>222</v>
+      </c>
+      <c r="M97" s="63">
+        <v>45413</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>223</v>
+      </c>
+      <c r="B98" t="s">
+        <v>227</v>
+      </c>
+      <c r="C98" t="s">
         <v>216</v>
       </c>
-      <c r="G92" t="s">
-        <v>218</v>
-      </c>
-      <c r="I92" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C93" t="s">
-        <v>220</v>
-      </c>
-      <c r="F93" t="s">
-        <v>222</v>
-      </c>
-      <c r="G93" t="s">
+      <c r="F98" t="s">
+        <v>224</v>
+      </c>
+      <c r="G98" t="s">
         <v>221</v>
       </c>
-      <c r="I93" t="s">
-        <v>212</v>
+      <c r="I98" t="s">
+        <v>225</v>
+      </c>
+      <c r="M98" s="63">
+        <v>45413</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Debugging last HH implementation
</commit_message>
<xml_diff>
--- a/pieces/Les pièces Skini.xlsx
+++ b/pieces/Les pièces Skini.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berpetit.AD\Documents\nodeskini\pieces\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berpetit\Documents\nodeskini\pieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781D17B9-19BD-47EE-B76D-B6380E3A6F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B37CF2-7379-47F8-A3E1-D7FCECE40811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26970" yWindow="-3000" windowWidth="25275" windowHeight="14805" xr2:uid="{6D6D9BFB-4BA4-4FFE-8AC7-F35E8058755B}"/>
+    <workbookView xWindow="-25920" yWindow="-180" windowWidth="21600" windowHeight="11325" xr2:uid="{6D6D9BFB-4BA4-4FFE-8AC7-F35E8058755B}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="235">
   <si>
     <t>opus1 skini V2-ABL10.als</t>
   </si>
@@ -733,6 +733,9 @@
   </si>
   <si>
     <t>Version du 30/5/2024</t>
+  </si>
+  <si>
+    <t>ATOMS3 arduino ATOMS3_OSC_Skini.ino</t>
   </si>
 </sst>
 </file>
@@ -1411,10 +1414,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3771670C-3569-4306-BADE-9BE1604036BE}">
   <dimension ref="A1:Y98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A12" sqref="A12"/>
-      <selection pane="topRight" activeCell="C108" sqref="C108"/>
+      <selection pane="topRight" activeCell="I93" sqref="I93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3154,6 +3157,9 @@
       <c r="G93" t="s">
         <v>210</v>
       </c>
+      <c r="I93" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C94" t="s">

</xml_diff>

<commit_message>
Debug HH and compilation
</commit_message>
<xml_diff>
--- a/pieces/Les pièces Skini.xlsx
+++ b/pieces/Les pièces Skini.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berpetit\Documents\nodeskini\pieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93B37CF2-7379-47F8-A3E1-D7FCECE40811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A54A4E94-C555-45A3-BD4B-5D89F56DF126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25920" yWindow="-180" windowWidth="21600" windowHeight="11325" xr2:uid="{6D6D9BFB-4BA4-4FFE-8AC7-F35E8058755B}"/>
+    <workbookView xWindow="2460" yWindow="732" windowWidth="21600" windowHeight="11328" xr2:uid="{6D6D9BFB-4BA4-4FFE-8AC7-F35E8058755B}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="247">
   <si>
     <t>opus1 skini V2-ABL10.als</t>
   </si>
@@ -736,6 +736,42 @@
   </si>
   <si>
     <t>ATOMS3 arduino ATOMS3_OSC_Skini.ino</t>
+  </si>
+  <si>
+    <t>EtudeSkiniHarmonie1</t>
+  </si>
+  <si>
+    <t>EtudeSkiniHarmonie2et3</t>
+  </si>
+  <si>
+    <t>EtudeSkiniHarmonie4</t>
+  </si>
+  <si>
+    <t>EtudeSkiniHarmonie5</t>
+  </si>
+  <si>
+    <t>EtudeSkiniHarmonie1.csv</t>
+  </si>
+  <si>
+    <t>EtudeSkiniHarmonie2.csv</t>
+  </si>
+  <si>
+    <t>EtudeSkiniHarmonie5.csv</t>
+  </si>
+  <si>
+    <t>EtudeSkiniHarmonie4.csv</t>
+  </si>
+  <si>
+    <t>EtudeSkiniHarmonie1.xml</t>
+  </si>
+  <si>
+    <t>EtudeSkiniHarmonie2et3.xml</t>
+  </si>
+  <si>
+    <t>EtudeSkiniHarmonie4.xml</t>
+  </si>
+  <si>
+    <t>EtudeSkiniHarmonie5.xml</t>
   </si>
 </sst>
 </file>
@@ -1412,12 +1448,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3771670C-3569-4306-BADE-9BE1604036BE}">
-  <dimension ref="A1:Y98"/>
+  <dimension ref="A1:Y102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A81" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A12" sqref="A12"/>
-      <selection pane="topRight" activeCell="I93" sqref="I93"/>
+      <selection pane="topRight" activeCell="C94" sqref="C94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3177,66 +3213,110 @@
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C95" t="s">
+        <v>239</v>
+      </c>
+      <c r="F95" t="s">
+        <v>235</v>
+      </c>
+      <c r="G95" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C96" t="s">
+        <v>240</v>
+      </c>
+      <c r="F96" t="s">
+        <v>236</v>
+      </c>
+      <c r="G96" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C97" t="s">
+        <v>242</v>
+      </c>
+      <c r="F97" t="s">
+        <v>237</v>
+      </c>
+      <c r="G97" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C98" t="s">
+        <v>241</v>
+      </c>
+      <c r="F98" t="s">
+        <v>238</v>
+      </c>
+      <c r="G98" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C99" t="s">
         <v>216</v>
       </c>
-      <c r="F95" t="s">
+      <c r="F99" t="s">
         <v>218</v>
       </c>
-      <c r="G95" t="s">
+      <c r="G99" t="s">
         <v>217</v>
       </c>
-      <c r="I95" t="s">
+      <c r="I99" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A96" s="61" t="s">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A100" s="61" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
         <v>220</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B101" t="s">
         <v>121</v>
       </c>
-      <c r="C97" t="s">
+      <c r="C101" t="s">
         <v>120</v>
       </c>
-      <c r="F97" t="s">
+      <c r="F101" t="s">
         <v>206</v>
       </c>
-      <c r="G97" t="s">
+      <c r="G101" t="s">
         <v>221</v>
       </c>
-      <c r="I97" t="s">
+      <c r="I101" t="s">
         <v>222</v>
       </c>
-      <c r="M97" s="63">
+      <c r="M101" s="63">
         <v>45413</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
         <v>223</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B102" t="s">
         <v>227</v>
       </c>
-      <c r="C98" t="s">
+      <c r="C102" t="s">
         <v>216</v>
       </c>
-      <c r="F98" t="s">
+      <c r="F102" t="s">
         <v>224</v>
       </c>
-      <c r="G98" t="s">
+      <c r="G102" t="s">
         <v>221</v>
       </c>
-      <c r="I98" t="s">
+      <c r="I102" t="s">
         <v>225</v>
       </c>
-      <c r="M98" s="63">
+      <c r="M102" s="63">
         <v>45413</v>
       </c>
     </row>

</xml_diff>

<commit_message>
test avec nouvelle version HH, plus de Blocky
</commit_message>
<xml_diff>
--- a/pieces/Les pièces Skini.xlsx
+++ b/pieces/Les pièces Skini.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berpetit\Documents\nodeskini\pieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A54A4E94-C555-45A3-BD4B-5D89F56DF126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31FA8B79-6D35-4205-8DD9-DFE37ABB359D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="732" windowWidth="21600" windowHeight="11328" xr2:uid="{6D6D9BFB-4BA4-4FFE-8AC7-F35E8058755B}"/>
+    <workbookView xWindow="-28920" yWindow="-3180" windowWidth="29040" windowHeight="15840" xr2:uid="{6D6D9BFB-4BA4-4FFE-8AC7-F35E8058755B}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -1450,10 +1450,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3771670C-3569-4306-BADE-9BE1604036BE}">
   <dimension ref="A1:Y102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A12" sqref="A12"/>
-      <selection pane="topRight" activeCell="C94" sqref="C94"/>
+      <selection pane="topRight" activeCell="G106" sqref="G106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1465,6 +1465,7 @@
     <col min="5" max="5" width="16.21875" customWidth="1"/>
     <col min="6" max="6" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="8" max="8" width="28.109375" customWidth="1"/>
     <col min="9" max="9" width="18.88671875" customWidth="1"/>
     <col min="10" max="10" width="16.5546875" customWidth="1"/>
     <col min="11" max="11" width="15.5546875" customWidth="1"/>

</xml_diff>

<commit_message>
programme de test hh.js
</commit_message>
<xml_diff>
--- a/pieces/Les pièces Skini.xlsx
+++ b/pieces/Les pièces Skini.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\berpetit\Documents\nodeskini\pieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31FA8B79-6D35-4205-8DD9-DFE37ABB359D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B59384A-2E60-4218-BE9E-B68DC96C9B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-3180" windowWidth="29040" windowHeight="15840" xr2:uid="{6D6D9BFB-4BA4-4FFE-8AC7-F35E8058755B}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="250">
   <si>
     <t>opus1 skini V2-ABL10.als</t>
   </si>
@@ -772,6 +772,15 @@
   </si>
   <si>
     <t>EtudeSkiniHarmonie5.xml</t>
+  </si>
+  <si>
+    <t>opus5.hh.js</t>
+  </si>
+  <si>
+    <t>opus1.hh.js</t>
+  </si>
+  <si>
+    <t>modIZetESP32HH.hh.js</t>
   </si>
 </sst>
 </file>
@@ -1448,12 +1457,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3771670C-3569-4306-BADE-9BE1604036BE}">
-  <dimension ref="A1:Y102"/>
+  <dimension ref="A1:Y106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A12" sqref="A12"/>
-      <selection pane="topRight" activeCell="G106" sqref="G106"/>
+      <selection pane="topRight" activeCell="C110" sqref="C110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3321,6 +3330,44 @@
         <v>45413</v>
       </c>
     </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>247</v>
+      </c>
+      <c r="C103" t="s">
+        <v>213</v>
+      </c>
+      <c r="M103" s="63">
+        <v>45992</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>248</v>
+      </c>
+      <c r="C104" t="s">
+        <v>25</v>
+      </c>
+      <c r="M104" s="63">
+        <v>46023</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>223</v>
+      </c>
+      <c r="C105" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>249</v>
+      </c>
+      <c r="C106" t="s">
+        <v>203</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>